<commit_message>
added sprint 3 and % of project
</commit_message>
<xml_diff>
--- a/Sprints.xlsx
+++ b/Sprints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexk\Documents\Schule\5\BSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexk\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t>Kogler</t>
   </si>
@@ -56,28 +56,115 @@
     <t>Sprint 2 (29.09 - 09.10)</t>
   </si>
   <si>
-    <t>GUI für Login, Register &amp; Forgot Password (WPF)</t>
-  </si>
-  <si>
-    <t>Entity Classes &amp; Program Logic for Login &amp; Register (WPF)</t>
-  </si>
-  <si>
-    <t>OleDB Aufrufe (Login, Register, Forgot Pw) &amp; Send E-Mail (WPF)</t>
-  </si>
-  <si>
-    <t>GUI für Login, Register, Forgot Password, Main &amp; Add Project (Android)</t>
-  </si>
-  <si>
-    <t>New Create Tables &amp; Trigger</t>
-  </si>
-  <si>
     <t>Datenmodell ausgebessert</t>
   </si>
   <si>
     <t>Filipovic, Kerschbaumer &amp; Kogler</t>
   </si>
   <si>
-    <t>New Entity Classes (WPF)</t>
+    <t>Sprint 3 (9.10 - 16.10)</t>
+  </si>
+  <si>
+    <t>JDBC Database connection (Insert User, Select Users)</t>
+  </si>
+  <si>
+    <t>Schiene</t>
+  </si>
+  <si>
+    <t>WPF-C#</t>
+  </si>
+  <si>
+    <t>Oracle Datenbank</t>
+  </si>
+  <si>
+    <t>GUI für Login, Register &amp; Forgot Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity Classes &amp; Program Logic for Login &amp; Register </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OleDB Aufrufe (Login, Register, Forgot Pw) &amp; Send E-Mail </t>
+  </si>
+  <si>
+    <t>Android-Java</t>
+  </si>
+  <si>
+    <t>GUI für Login, Register, Forgot Password, Main &amp; Add Project</t>
+  </si>
+  <si>
+    <t>Oracle-Datenbank</t>
+  </si>
+  <si>
+    <t>Er-Diagramm</t>
+  </si>
+  <si>
+    <t>GUI changes in Main(Navigation, List), Add Project</t>
+  </si>
+  <si>
+    <t>Neue Create Tables &amp; Trigger</t>
+  </si>
+  <si>
+    <t>Neue Datenmodell (Gruppen wurden gelöscht und Fehler behoben)</t>
+  </si>
+  <si>
+    <t>Filipovic, Kerschbaumer</t>
+  </si>
+  <si>
+    <t>Neue Entity Classes (Rollen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neue Entity Classes </t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Forgot Pw</t>
+  </si>
+  <si>
+    <t>Main (Show Project)</t>
+  </si>
+  <si>
+    <t>OleDB Calls</t>
+  </si>
+  <si>
+    <t>Show Profile</t>
+  </si>
+  <si>
+    <t>Show Sprints</t>
+  </si>
+  <si>
+    <t>Show Issues</t>
+  </si>
+  <si>
+    <t>Add Projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Sprints </t>
+  </si>
+  <si>
+    <t>Add Issues</t>
+  </si>
+  <si>
+    <t>Add Roles</t>
+  </si>
+  <si>
+    <t>Gesammt</t>
+  </si>
+  <si>
+    <t>Entity Classes</t>
+  </si>
+  <si>
+    <t>MongoDB</t>
+  </si>
+  <si>
+    <t>Spatial</t>
+  </si>
+  <si>
+    <t>JDBC Calls</t>
   </si>
 </sst>
 </file>
@@ -121,12 +208,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -409,124 +499,457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="F17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="4">
+        <f>AVERAGE(G2:G16)</f>
+        <v>0.3</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="4">
+        <f>AVERAGE(I2:I16)</f>
+        <v>0.32666666666666672</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C22" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A9:B9"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>